<commit_message>
added missing nmr software:
Open source nmr data visualizers
metaboquant (Matlab-based)
Batman R package
rNMR
MetaboMiner
Sparky - NMR Assignment and Integration Software
ACD/NMR Processor Academic Edition
Rowland nmr tools
X-PLOR A System for X-ray Crystallography and NMR
Spinach, a fast (polynomially scaling) open-source Liouville space spin dynamics simulation library.
Commercial nmr software
nmrPipe
ACD NMR Software
iNMR
MestReNova (Mnova)
nuts
Rowland NMR Toolkit
Felix Nmr
ScienceSoft's NMR Software Site
Vendor software
Bruker Topspin
Agilent Vnmr
Jeol Delta
Link collections on nmr tools
http://nmrwiki.org/wiki/index.php?title=Online_data_tools
http://nmr-software.blogspot.de/
http://spincore.com/nmrinfo/
http://www.cgl.ucsf.edu/home/sparky/nmrlinks.html
Converters & Parsers
WeNMR converter
XSDs
SpinXML
aniML
</commit_message>
<xml_diff>
--- a/tools/MajorNMRTools.xlsx
+++ b/tools/MajorNMRTools.xlsx
@@ -1,32 +1,228 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Existing Visualizers, Parsers, convertors, xslt, Validators, …</t>
-  </si>
-  <si>
-    <t>Existing Vendor software</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://www1.imperial.ac.uk/resources/C336E14F-D8F6-4411-AD84-7985DE780723/batman1.0.9.05.pdf</t>
+  </si>
+  <si>
+    <t>Batman R package</t>
+  </si>
+  <si>
+    <t>paper URL</t>
+  </si>
+  <si>
+    <t>rNMR</t>
+  </si>
+  <si>
+    <t>metaboquant (Matlab-based)</t>
+  </si>
+  <si>
+    <t>http://genomics.uni-regensburg.de/site/institute/software/metaboquant</t>
+  </si>
+  <si>
+    <t>http://bioinformatics.oxfordjournals.org/content/early/2012/05/25/bioinformatics.bts308.short?rss=1</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pmc/articles/PMC2798074/pdf/mrc0047-S123.pdf</t>
+  </si>
+  <si>
+    <t>iNMR</t>
+  </si>
+  <si>
+    <t>http://www.inmr.net/articles/index.html</t>
+  </si>
+  <si>
+    <t>MestReNova (Mnova)</t>
+  </si>
+  <si>
+    <t>http://mestrelab.com/</t>
+  </si>
+  <si>
+    <t>nuts</t>
+  </si>
+  <si>
+    <t>http://www.acornnmr.com/nuts.htm</t>
+  </si>
+  <si>
+    <t>nmrPipe</t>
+  </si>
+  <si>
+    <t>http://spin.niddk.nih.gov/NMRPipe/</t>
+  </si>
+  <si>
+    <t>Rowland NMR Toolkit</t>
+  </si>
+  <si>
+    <t>http://rnmrtk.uchc.edu/rnmrtk/RNMRTK.html</t>
+  </si>
+  <si>
+    <t>Bruker Topspin</t>
+  </si>
+  <si>
+    <t>http://www.bruker.com/products/magnetic-resonance/nmr/sw/nmr-software/topspin/overview.html</t>
+  </si>
+  <si>
+    <t>Agilent Vnmr</t>
+  </si>
+  <si>
+    <t>http://www.chem.agilent.com/en-US/products-services/software-informatics/vnmrj-30/Pages/default.aspx</t>
+  </si>
+  <si>
+    <t>Jeol Delta</t>
+  </si>
+  <si>
+    <t>http://www.jeol.com/PRODUCTS/AnalyticalInstruments/NuclearMagneticResonance/DeltaNMRSoftware/tabid/395/Default.aspx</t>
+  </si>
+  <si>
+    <t>Commercial nmr software</t>
+  </si>
+  <si>
+    <t>Open source nmr data visualizers</t>
+  </si>
+  <si>
+    <t>Vendor software</t>
+  </si>
+  <si>
+    <t>i/o FILE FORMATS</t>
+  </si>
+  <si>
+    <t>Support Contact</t>
+  </si>
+  <si>
+    <t>unique key feature of that software that COSMOS is interested in</t>
+  </si>
+  <si>
+    <t>http://www.felixnmr.com/</t>
+  </si>
+  <si>
+    <t>Felix Nmr</t>
+  </si>
+  <si>
+    <t>ScienceSoft's NMR Software Site</t>
+  </si>
+  <si>
+    <t>http://www.sciencesoft.net/</t>
+  </si>
+  <si>
+    <t>http://nmrwiki.org/wiki/index.php?title=Online_data_tools</t>
+  </si>
+  <si>
+    <t>http://nmr-software.blogspot.de/</t>
+  </si>
+  <si>
+    <t>http://spincore.com/nmrinfo/</t>
+  </si>
+  <si>
+    <t>http://www.cgl.ucsf.edu/home/sparky/nmrlinks.html</t>
+  </si>
+  <si>
+    <t>MetaboMiner</t>
+  </si>
+  <si>
+    <t>To aid in rapid and efficient metabolite identification from complex mixtures using 2D NMR spectroscopy</t>
+  </si>
+  <si>
+    <t>http://wishart.biology.ualberta.ca/metabominer/</t>
+  </si>
+  <si>
+    <t>Programming Language</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>http://www.cgl.ucsf.edu/home/sparky/</t>
+  </si>
+  <si>
+    <t>Sparky - NMR Assignment and Integration Software</t>
+  </si>
+  <si>
+    <t>http://www.acdlabs.com/resources/freeware/nmr_proc/index.php</t>
+  </si>
+  <si>
+    <t>http://www.acdlabs.com/products/adh/nmr/</t>
+  </si>
+  <si>
+    <t>http://sbtools.uchc.edu/nmr/</t>
+  </si>
+  <si>
+    <t>ACD/NMR Processor Academic Edition</t>
+  </si>
+  <si>
+    <t>ACD NMR Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X-PLOR A System for X-ray Crystallography and NMR </t>
+  </si>
+  <si>
+    <t>http://nmr.cit.nih.gov/xplor-nih/doc/current/</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>very old</t>
+  </si>
+  <si>
+    <t>Rowland nmr tools</t>
+  </si>
+  <si>
+    <t>Converters &amp; Parsers</t>
+  </si>
+  <si>
+    <t>http://www.wenmr.eu/wenmr/formatconverter-walk-through</t>
+  </si>
+  <si>
+    <t>WeNMR converter</t>
+  </si>
+  <si>
+    <t>Link collections on nmr tools</t>
+  </si>
+  <si>
+    <t>Spinach, a fast (polynomially scaling) open-source Liouville space spin dynamics simulation library.</t>
+  </si>
+  <si>
+    <t>http://spindynamics.org/Spinach.php</t>
+  </si>
+  <si>
+    <t>XSDs</t>
+  </si>
+  <si>
+    <t>http://spindynamics.org/SpinXML.php</t>
+  </si>
+  <si>
+    <t>SpinXML</t>
+  </si>
+  <si>
+    <t>aniML</t>
+  </si>
+  <si>
+    <t>ccpn based data converter from WeNMR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,6 +235,45 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -58,16 +293,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -126,7 +379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -161,7 +414,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,32 +623,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection sqref="A1:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="B15" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added software and links
</commit_message>
<xml_diff>
--- a/tools/MajorNMRTools.xlsx
+++ b/tools/MajorNMRTools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>URL</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>ccpn based data converter from WeNMR</t>
+  </si>
+  <si>
+    <t>http://animl.sourceforge.net/</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:A38"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,6 +910,9 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>65</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates some software and vendor formats (sheet 2)
</commit_message>
<xml_diff>
--- a/tools/MajorNMRTools.xlsx
+++ b/tools/MajorNMRTools.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="NMRtools" sheetId="1" r:id="rId1"/>
+    <sheet name="VendorFormats&amp;Files" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
   <si>
     <t>URL</t>
   </si>
@@ -219,6 +219,153 @@
   </si>
   <si>
     <t>http://animl.sourceforge.net/</t>
+  </si>
+  <si>
+    <t>CcpNmr Analysis</t>
+  </si>
+  <si>
+    <t>http://www.ccpn.ac.uk/software/analysis</t>
+  </si>
+  <si>
+    <t>CcpNmr SpecView</t>
+  </si>
+  <si>
+    <t>http://www.ccpn.ac.uk/software/specview</t>
+  </si>
+  <si>
+    <t>CcpNmr ChemBuild</t>
+  </si>
+  <si>
+    <t>http://www.ccpn.ac.uk/software/chembuild</t>
+  </si>
+  <si>
+    <t>CcpNmr FormatExchange</t>
+  </si>
+  <si>
+    <t>http://www.ccpn.ac.uk/software/format-exchange</t>
+  </si>
+  <si>
+    <t>CcpNmr FormatConverter</t>
+  </si>
+  <si>
+    <t>http://www.ccpn.ac.uk/software/fcfolder</t>
+  </si>
+  <si>
+    <t>The CCPN Data Model for macromolecular NMR is intended to cover all data needed for macromolecular NMR spectroscopy from the initial experimental data to the final validation. It serves for exchange of data between programs, for storage, data harvesting, and database deposition. The data model proper is an abstract description of the relevant data and their relationships - it is implemented in the modeling language UML. From this CCPN autogenerates interfaces (APIs) for various languages, format description and I/O routines, and documentation</t>
+  </si>
+  <si>
+    <t>Other formats and APIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCPN </t>
+  </si>
+  <si>
+    <t>http://www.ccpn.ac.uk/software/extras/datamodelfolder/datamodel</t>
+  </si>
+  <si>
+    <t>NMR data formats listed on http://www.acdlabs.com/products/fileformats/</t>
+  </si>
+  <si>
+    <t>NMR Vendor</t>
+  </si>
+  <si>
+    <t>File Format</t>
+  </si>
+  <si>
+    <t>Required Parameter Files</t>
+  </si>
+  <si>
+    <t>Optional Parameter Files</t>
+  </si>
+  <si>
+    <t>ACD/Labs, Inc.</t>
+  </si>
+  <si>
+    <t>*.esp, *.txt</t>
+  </si>
+  <si>
+    <t>Acorn NMR, Inc.</t>
+  </si>
+  <si>
+    <t>*.fid, *.nmr, *.2d</t>
+  </si>
+  <si>
+    <t>ASCII†</t>
+  </si>
+  <si>
+    <t>*.txt; *.prn, *.csv, *.asc</t>
+  </si>
+  <si>
+    <t>Bruker Corporation</t>
+  </si>
+  <si>
+    <t>ser, rr, .fid, *r, 1i, 2rr,</t>
+  </si>
+  <si>
+    <t>acqus, procs, acqu2, proc2s, *.fqs, *.fa1, *.fa2, *.fp1, *.fp2</t>
+  </si>
+  <si>
+    <t>title, intrng, *.tit, *.ti2</t>
+  </si>
+  <si>
+    <t>*.* (DISNMR)</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>*.raw, *.* (Nicolet)</t>
+  </si>
+  <si>
+    <t>JCAMP†</t>
+  </si>
+  <si>
+    <t>*.dx; *.jdx</t>
+  </si>
+  <si>
+    <t>JEOL Ltd.</t>
+  </si>
+  <si>
+    <t>*.als, *.nmfid, *.nmf, *.nmdata, *.nmd, *.gxd, *.bin, *.* (Delta)</t>
+  </si>
+  <si>
+    <t>*.gxp, *.hdr</t>
+  </si>
+  <si>
+    <t>exp.param, exp.par</t>
+  </si>
+  <si>
+    <t>Lybrics</t>
+  </si>
+  <si>
+    <t>*.*</t>
+  </si>
+  <si>
+    <t>MSI Felix</t>
+  </si>
+  <si>
+    <t>Tecmag</t>
+  </si>
+  <si>
+    <t>*.tnt, *.* (MacNMR)</t>
+  </si>
+  <si>
+    <t>Thermo Scientific†</t>
+  </si>
+  <si>
+    <t>*.spc</t>
+  </si>
+  <si>
+    <t>Varian, Inc.</t>
+  </si>
+  <si>
+    <t>data, *.fdf, fid0001.fdf, *.txt, fid, phasefile</t>
+  </si>
+  <si>
+    <t>acq, proc, procpar</t>
+  </si>
+  <si>
+    <t>acq_2, text</t>
   </si>
 </sst>
 </file>
@@ -300,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -321,9 +468,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -417,7 +573,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +797,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -752,175 +908,322 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>50</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
+      <c r="A19" t="s">
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>27</v>
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="B15" r:id="rId2"/>
+    <hyperlink ref="B18" r:id="rId2"/>
     <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B14" r:id="rId4"/>
+    <hyperlink ref="B17" r:id="rId4"/>
     <hyperlink ref="B9" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -930,12 +1233,182 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added further nmr tools and APIs
</commit_message>
<xml_diff>
--- a/tools/MajorNMRTools.xlsx
+++ b/tools/MajorNMRTools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="175">
   <si>
     <t>URL</t>
   </si>
@@ -56,15 +56,9 @@
     <t>http://mestrelab.com/</t>
   </si>
   <si>
-    <t>nuts</t>
-  </si>
-  <si>
     <t>http://www.acornnmr.com/nuts.htm</t>
   </si>
   <si>
-    <t>nmrPipe</t>
-  </si>
-  <si>
     <t>http://spin.niddk.nih.gov/NMRPipe/</t>
   </si>
   <si>
@@ -381,6 +375,171 @@
   </si>
   <si>
     <t>http://connjur.uchc.edu/</t>
+  </si>
+  <si>
+    <t>http://www.metexplore.fr/</t>
+  </si>
+  <si>
+    <t>Metexplore</t>
+  </si>
+  <si>
+    <t>Metabolomics related Databases</t>
+  </si>
+  <si>
+    <t>Metabolomics Access Portals and Hubs</t>
+  </si>
+  <si>
+    <t>Higher order Tools we might integrate with</t>
+  </si>
+  <si>
+    <t>R/Bioconductor</t>
+  </si>
+  <si>
+    <t>Matlab</t>
+  </si>
+  <si>
+    <t>http://www.bioconductor.org/</t>
+  </si>
+  <si>
+    <t>ISA tab 2 RDF (by Toxbank group)</t>
+  </si>
+  <si>
+    <t>http://www.smpdb.ca/about</t>
+  </si>
+  <si>
+    <t>smpdb</t>
+  </si>
+  <si>
+    <t>Small molecule Pathways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A web server to link metabolomic experiments and genome-scale metabolic networks. MetExplore stores metabolic networks of 160 organisms into a relational database (freely available on demand). Information about metabolic networks mainly come from BioCyc-like databases. Two BioCyc-like databases contain information about several organisms: PlantCyc and MetaCyc. MetExplore contains also the information about metabolites stored in Metabolome.jp. Note that there is no information about reactions in this database and is only useful to identify compounds from masses. Several genome-scale models designed for Flux Balance Analysis have also been imported into MetExplore.MetExplore is able to deal with data from metabolomics experiments by mapping a list of masses or identifiers onto filtered metabolic networks. </t>
+  </si>
+  <si>
+    <t>CML</t>
+  </si>
+  <si>
+    <t>http://www.xml-cml.org/spec/</t>
+  </si>
+  <si>
+    <t>CML (Chemical Markup Language) is an XML language designed to hold most of the central concepts in chemistry. It was the first language to be developed and plays the same role for chemistry as MathML for mathematics and GML for geographical systems. CML covers most mainstream chemistry and especially molecules, reactions, solid-state, computation and spectroscopy. Since it has a special flexible approach to numeric science it also covers a very wide range of chemical properties, parameters and experimental observation.</t>
+  </si>
+  <si>
+    <t>Birmingham Conversion tools: Bruker import into DTB (python), DTB 2 rubtsov XML (Java)</t>
+  </si>
+  <si>
+    <t>Nuts</t>
+  </si>
+  <si>
+    <t>Chenomx NMR Suite</t>
+  </si>
+  <si>
+    <t>http://www.chenomx.com/software/</t>
+  </si>
+  <si>
+    <t>An integrated set of tools for identifying and quantifying metabolites in NMR spectra.</t>
+  </si>
+  <si>
+    <t>NmrPipe</t>
+  </si>
+  <si>
+    <t>Metassimulo</t>
+  </si>
+  <si>
+    <t>http://cisbic.bioinformatics.ic.ac.uk/metassimulo/</t>
+  </si>
+  <si>
+    <t>A MATLAB-based package which simulates 1H-NMR spectra of complex mixtures such as metabolic profiles. Drawing data from a metabolite standard spectral database in conjunction with concentration information input by the user or constructed automatically from the Human Metabolome Database, MetAssimulo is able to create realistic metabolic profiles containing large numbers of metabolites with a range of user-defined properties. Current features include the simulation of two groups ('case' and 'control') specified by means and standard deviations of concentrations for each metabolite.</t>
+  </si>
+  <si>
+    <t>Baysian statistics for metabolite fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">very complex, not really supported anymore </t>
+  </si>
+  <si>
+    <t>Jcamp-DX</t>
+  </si>
+  <si>
+    <t>http://www.jcamp-dx.org/</t>
+  </si>
+  <si>
+    <t>Role-model tools that show hoe xml/CV can be semantically exploited</t>
+  </si>
+  <si>
+    <t>http://validator.xml-cml.org/</t>
+  </si>
+  <si>
+    <t>CML Validator</t>
+  </si>
+  <si>
+    <t>Free xml Editors</t>
+  </si>
+  <si>
+    <t>http://www.freexmleditorsite.com/download.html</t>
+  </si>
+  <si>
+    <t>http://en.wikipedia.org/wiki/CAM_editor</t>
+  </si>
+  <si>
+    <t>CAM editor</t>
+  </si>
+  <si>
+    <t>Free editix</t>
+  </si>
+  <si>
+    <t>http://www.bml-nmr.org</t>
+  </si>
+  <si>
+    <t>http://www.nmrlab.org.uk</t>
+  </si>
+  <si>
+    <t>nmrLab</t>
+  </si>
+  <si>
+    <t>A software package for NMR processing written in MATLAB currently developed at the University of Birmingham. It contains of a series of processing algorithms for 1D, 2D and 3D processing including apodization functions, linear prediction, Fourier transformation, baseline correction. It also includes routines for wavelet denoising of spectra. A simple interface is available to set up processing parameters. The current version supports Bruker and Varian file formats.</t>
+  </si>
+  <si>
+    <t>MetaboLab</t>
+  </si>
+  <si>
+    <t>MetaboLab is an extension of NMRLab for metabolomics post-processing. It includes routines for Bruker and Varian data, including alignment tools, various scaling algorithms (autoscale, Pareto scaling and glog transform), graphical selection of exclusion regions, bucketing, wavelet de-noising algorithms and links to PCA and PLS algorithms.NMRKIN is a related package for simulating line shapes derived from two-dimensional spectra in proteins.</t>
+  </si>
+  <si>
+    <t>Pride Inspector</t>
+  </si>
+  <si>
+    <t>http://www.nature.com/nbt/journal/v30/n2/full/nbt.2112.html</t>
+  </si>
+  <si>
+    <t>We want something like this, but für NMR</t>
+  </si>
+  <si>
+    <t>http://services.cbib.u-bordeaux2.fr/SPECNMR/run/example</t>
+  </si>
+  <si>
+    <t>Spectra overlay for NMR</t>
+  </si>
+  <si>
+    <t>http://services.cbib.u-bordeaux2.fr/MERYB/</t>
+  </si>
+  <si>
+    <t>MeRy-B</t>
+  </si>
+  <si>
+    <t>MeRy-B is a plant metabolomics knowledgebase allowing the storage and visualisation of metabolic profiles from plants</t>
+  </si>
+  <si>
+    <t>Less relevant Vendor formats</t>
+  </si>
+  <si>
+    <t>Acorn_NMR_Inc, Doty_Scientific,  JS_Research, MR_Resources, tecmag, Wilmad, …</t>
+  </si>
+  <si>
+    <t>http://www.nmrtec.com/index.php?option=com_kunena&amp;Itemid=190&amp;func=showcat&amp;catid=7</t>
+  </si>
+  <si>
+    <t>NMRTec nmrNotebook</t>
   </si>
 </sst>
 </file>
@@ -468,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -500,6 +659,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -805,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +999,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -831,19 +1008,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -864,7 +1041,9 @@
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -876,403 +1055,615 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="11"/>
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>72</v>
       </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>74</v>
       </c>
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B53" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="12"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>119</v>
-      </c>
-      <c r="B40" s="11" t="s">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="B71" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="9"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
+      <c r="D71" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
+  <mergeCells count="2">
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="B18" r:id="rId2"/>
+    <hyperlink ref="B23" r:id="rId2"/>
     <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B17" r:id="rId4"/>
+    <hyperlink ref="B22" r:id="rId4"/>
     <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B60" r:id="rId6"/>
+    <hyperlink ref="B59" r:id="rId7"/>
+    <hyperlink ref="B76" r:id="rId8"/>
+    <hyperlink ref="B80" r:id="rId9"/>
+    <hyperlink ref="B81" r:id="rId10"/>
+    <hyperlink ref="B56" r:id="rId11" display="http://www.bml-nmr.org/"/>
+    <hyperlink ref="B15" r:id="rId12" display="http://www.nmrlab.org.uk/"/>
+    <hyperlink ref="B16" r:id="rId13" display="http://www.nmrlab.org.uk/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -1288,7 +1679,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1296,156 +1687,156 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="D6" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="10" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Mani Pine Server	http://pine.nmrfam.wisc.edu/
</commit_message>
<xml_diff>
--- a/tools/MajorNMRTools.xlsx
+++ b/tools/MajorNMRTools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="180">
   <si>
     <t>URL</t>
   </si>
@@ -119,9 +119,6 @@
     <t>http://nmrwiki.org/wiki/index.php?title=Online_data_tools</t>
   </si>
   <si>
-    <t>http://nmr-software.blogspot.de/</t>
-  </si>
-  <si>
     <t>http://spincore.com/nmrinfo/</t>
   </si>
   <si>
@@ -540,13 +537,31 @@
   </si>
   <si>
     <t>NMRTec nmrNotebook</t>
+  </si>
+  <si>
+    <t>Au programs can be used to convert spectra (both FID’s or processed data files) as ASCII files</t>
+  </si>
+  <si>
+    <t>Although the JCAMP-DX export format has been largely used, it does not possess a flexible hierarchical structure and is not easily extendable for capturing supplementary information (e.g. outputs such as buckets or molecular structures). Such extensability, i.e. as shown in XML formats such as AnIML (http://animl.sourceforge.net/) or CMLspect is a highly desired feature of the standard we intent to develop</t>
+  </si>
+  <si>
+    <t>Mani Pine Server</t>
+  </si>
+  <si>
+    <t>http://pine.nmrfam.wisc.edu/</t>
+  </si>
+  <si>
+    <t>Probabilistic Interaction Network of Evidence Algorithm and its Application to Complete Labeling of Peak lists from Protein NMR Spectroscopy. PINE accepts, as input, the sequence of the protein plus peak lists (or spin systems) from a variety of NMR experiments and offers automatic backbone and sidechain assignments, detection and automated correction of potential referencing problems or inconsistent assignments and secondary structure determination.</t>
+  </si>
+  <si>
+    <t>most links are outdated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +605,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -612,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -628,9 +649,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -650,12 +668,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -964,7 +986,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +999,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -987,13 +1009,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>27</v>
@@ -1011,7 +1033,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1021,11 +1043,11 @@
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1034,128 +1056,136 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B17" s="9" t="s">
         <v>166</v>
       </c>
+      <c r="B17" s="8" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
+      <c r="A18" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1164,7 +1194,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>14</v>
@@ -1172,10 +1202,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,7 +1226,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>13</v>
@@ -1228,21 +1258,21 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1250,7 +1280,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>17</v>
       </c>
@@ -1258,7 +1288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>19</v>
       </c>
@@ -1266,7 +1296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>21</v>
       </c>
@@ -1274,189 +1304,196 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>36</v>
+      <c r="D47" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>54</v>
+      <c r="A50" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>118</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D56" s="10"/>
+        <v>135</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" s="9"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="D61" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="D62" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="B64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="D65" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>148</v>
+      <c r="D66" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,152 +1501,152 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="5" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
+      <c r="A78" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
+      <c r="A79" s="11"/>
+      <c r="B79" s="11"/>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="12" t="s">
-        <v>156</v>
+      <c r="A81" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="B81" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
+      <c r="A89" s="11"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
+      <c r="A90" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1633,7 +1670,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1641,156 +1678,156 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MFB NMR viewer
</commit_message>
<xml_diff>
--- a/tools/MajorNMRTools.xlsx
+++ b/tools/MajorNMRTools.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="22470" windowHeight="10485"/>
   </bookViews>
   <sheets>
     <sheet name="NMRtools" sheetId="1" r:id="rId1"/>
     <sheet name="VendorFormats&amp;Files" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
   <si>
     <t>URL</t>
   </si>
@@ -512,12 +512,6 @@
     <t>We want something like this, but für NMR</t>
   </si>
   <si>
-    <t>http://services.cbib.u-bordeaux2.fr/SPECNMR/run/example</t>
-  </si>
-  <si>
-    <t>Spectra overlay for NMR</t>
-  </si>
-  <si>
     <t>http://services.cbib.u-bordeaux2.fr/MERYB/</t>
   </si>
   <si>
@@ -555,13 +549,22 @@
   </si>
   <si>
     <t>most links are outdated</t>
+  </si>
+  <si>
+    <t>MFB NMR viewer</t>
+  </si>
+  <si>
+    <t>https://github.com/nmrML/nmrML/tree/master/tools/Visualizers/PMB_NMRviewer</t>
+  </si>
+  <si>
+    <t>See http://www.cbib.u-bordeaux2.fr/SPECNMR/test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -671,17 +674,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -697,9 +703,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -737,9 +743,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -771,10 +777,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -806,10 +811,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -982,14 +986,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H90"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="61.140625" style="5" customWidth="1"/>
@@ -998,7 +1002,7 @@
     <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
@@ -1068,7 +1072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
@@ -1076,7 +1080,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -1084,7 +1088,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
         <v>52</v>
       </c>
@@ -1092,7 +1096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -1103,7 +1107,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
         <v>57</v>
       </c>
@@ -1111,7 +1115,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
         <v>65</v>
       </c>
@@ -1119,7 +1123,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -1127,7 +1131,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
         <v>69</v>
       </c>
@@ -1135,7 +1139,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
         <v>141</v>
       </c>
@@ -1146,7 +1150,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
         <v>158</v>
       </c>
@@ -1157,7 +1161,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
         <v>160</v>
       </c>
@@ -1168,507 +1172,520 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="9"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" s="9"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B74" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="9"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B64" s="8"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B73" s="5" t="s">
+      <c r="D74" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="10"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    </row>
+    <row r="76" spans="1:4">
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B77" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B78" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C77" s="11"/>
-      <c r="D77" s="5" t="s">
+      <c r="C78" s="11"/>
+      <c r="D78" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
+    <row r="79" spans="1:4">
+      <c r="A79" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
       <c r="B79" s="11"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="11"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B82" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B82" s="11"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+    <row r="83" spans="1:4">
+      <c r="A83" s="11" t="s">
+        <v>154</v>
+      </c>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="11"/>
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="11"/>
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="11"/>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="11"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="11"/>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -1676,7 +1693,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -1690,7 +1707,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="4" t="s">
         <v>84</v>
       </c>
@@ -1700,7 +1717,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="4" t="s">
         <v>86</v>
       </c>
@@ -1710,7 +1727,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="4" t="s">
         <v>88</v>
       </c>
@@ -1720,29 +1737,29 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="15" t="s">
         <v>90</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:4" ht="30">
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" ht="30">
       <c r="A8" s="4" t="s">
         <v>95</v>
       </c>
@@ -1752,7 +1769,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
         <v>97</v>
       </c>
@@ -1762,7 +1779,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="120">
       <c r="A10" s="4" t="s">
         <v>99</v>
       </c>
@@ -1776,7 +1793,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
         <v>103</v>
       </c>
@@ -1786,7 +1803,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
         <v>105</v>
       </c>
@@ -1796,7 +1813,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="4" t="s">
         <v>106</v>
       </c>
@@ -1806,7 +1823,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" s="4" t="s">
         <v>108</v>
       </c>
@@ -1816,7 +1833,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="60">
       <c r="A15" s="4" t="s">
         <v>110</v>
       </c>

</xml_diff>